<commit_message>
add some constrains for xlsx parsing add check if course id in xlsx match the course selected
</commit_message>
<xml_diff>
--- a/project2/tetris3D/download/demo.xlsx
+++ b/project2/tetris3D/download/demo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
   <si>
     <t>浙江大学课程考试成绩记录表</t>
   </si>
@@ -28,25 +28,28 @@
     <t>课程编号</t>
   </si>
   <si>
+    <t>00000002</t>
+  </si>
+  <si>
+    <t>学号</t>
+  </si>
+  <si>
+    <t>姓名</t>
+  </si>
+  <si>
+    <t>成绩</t>
+  </si>
+  <si>
+    <t>备注</t>
+  </si>
+  <si>
+    <t>0000000001</t>
+  </si>
+  <si>
+    <t>zhazha</t>
+  </si>
+  <si>
     <t>0000000002</t>
-  </si>
-  <si>
-    <t>学号</t>
-  </si>
-  <si>
-    <t>姓名</t>
-  </si>
-  <si>
-    <t>成绩</t>
-  </si>
-  <si>
-    <t>备注</t>
-  </si>
-  <si>
-    <t>0000000001</t>
-  </si>
-  <si>
-    <t>zhazha</t>
   </si>
   <si>
     <t>hahaha</t>
@@ -396,8 +399,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:sheetPr xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
     <s:outlinePr summaryBelow="1" summaryRight="1"/>
     <s:pageSetUpPr/>
   </s:sheetPr>
@@ -410,7 +413,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+      <c s="1" r="A1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -459,10 +462,10 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7" t="n">
         <v>77.5</v>
@@ -470,10 +473,10 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" t="n">
         <v>66.5</v>
@@ -481,10 +484,10 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" t="n">
         <v>99.5</v>

</xml_diff>

<commit_message>
fix a bug with 'Class_info' when upload xlsx file
</commit_message>
<xml_diff>
--- a/project2/tetris3D/download/demo.xlsx
+++ b/project2/tetris3D/download/demo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
   <si>
     <t>浙江大学课程考试成绩记录表</t>
   </si>
@@ -28,7 +28,7 @@
     <t>课程编号</t>
   </si>
   <si>
-    <t>00000002</t>
+    <t>00000004</t>
   </si>
   <si>
     <t>学号</t>
@@ -41,18 +41,6 @@
   </si>
   <si>
     <t>备注</t>
-  </si>
-  <si>
-    <t>0000000001</t>
-  </si>
-  <si>
-    <t>zhazha</t>
-  </si>
-  <si>
-    <t>0000000002</t>
-  </si>
-  <si>
-    <t>hahaha</t>
   </si>
   <si>
     <t>0000000003</t>
@@ -404,7 +392,7 @@
     <s:outlinePr summaryBelow="1" summaryRight="1"/>
     <s:pageSetUpPr/>
   </s:sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -412,85 +400,57 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c s="1" r="A1" t="s">
+    <row spans="1:6" r="1">
+      <c s="1" t="s" r="A1">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6"/>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
+    <row spans="1:6" r="2"/>
+    <row spans="1:6" r="3">
+      <c t="s" r="A3">
         <v>1</v>
       </c>
-      <c r="B3" t="s"/>
-      <c r="C3" t="s">
+      <c t="s" r="B3"/>
+      <c t="s" r="C3">
         <v>2</v>
       </c>
-      <c r="D3" t="s"/>
-      <c r="E3" t="s">
+      <c t="s" r="D3"/>
+      <c t="s" r="E3">
         <v>3</v>
       </c>
-      <c r="F3" t="s">
+      <c t="s" r="F3">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6"/>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
+    <row spans="1:6" r="4"/>
+    <row spans="1:6" r="5">
+      <c t="s" r="A5">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c t="s" r="B5">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
+      <c t="s" r="C5">
         <v>7</v>
       </c>
-      <c r="D5" t="s">
+      <c t="s" r="D5">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
+    <row spans="1:6" r="6">
+      <c t="s" r="A6">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c t="s" r="B6">
         <v>10</v>
       </c>
-      <c r="C6" t="n">
-        <v>88.5</v>
-      </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
+    <row spans="1:6" r="7">
+      <c t="s" r="A7">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
+      <c t="s" r="B7">
         <v>12</v>
-      </c>
-      <c r="C7" t="n">
-        <v>77.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="n">
-        <v>66.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="n">
-        <v>99.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>